<commit_message>
agregado OBSERVACIONES de los estudiantes de maestria y correccion en AddEstDoctForm
</commit_message>
<xml_diff>
--- a/PosgrIQ/bin/Release/templates/templateEstudiantesMaes.xlsx
+++ b/PosgrIQ/bin/Release/templates/templateEstudiantesMaes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>TABLA DE ESTUDIANTES DE MAESTRIA</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>CONCEPTO</t>
+  </si>
+  <si>
+    <t>NIVEL</t>
   </si>
 </sst>
 </file>
@@ -130,12 +133,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -165,7 +177,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2501272</xdr:colOff>
+      <xdr:colOff>2215522</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>91442</xdr:rowOff>
     </xdr:to>
@@ -469,17 +481,17 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:N11"/>
+  <dimension ref="A2:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="44.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
     <col min="4" max="4" width="48.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="6" max="6" width="24.7109375" customWidth="1"/>
@@ -491,61 +503,103 @@
     <col min="15" max="15" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D2" s="3"/>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="C22" s="6"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D11" s="4"/>
+      <c r="C23" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="37" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
listos los tres primeros informes
</commit_message>
<xml_diff>
--- a/PosgrIQ/bin/Release/templates/templateEstudiantesMaes.xlsx
+++ b/PosgrIQ/bin/Release/templates/templateEstudiantesMaes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PosgrIQ\PosgrIQ\bin\Release\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hdsp\Dropbox\Posgrados Ing Quimica\PosgrIQ\PosgrIQ\bin\Release\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,7 +135,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2215522</xdr:colOff>
+      <xdr:colOff>1701172</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>91442</xdr:rowOff>
     </xdr:to>
@@ -144,7 +144,7 @@
         <xdr:cNvPr id="4" name="Imagen 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -255,23 +255,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -307,23 +290,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -482,13 +448,13 @@
   <dimension ref="A2:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="B6" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
     <col min="3" max="3" width="42.140625" customWidth="1"/>
     <col min="4" max="4" width="48.7109375" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
listo el segundo grupo de informes, pero se debe revisar Directores
</commit_message>
<xml_diff>
--- a/PosgrIQ/bin/Release/templates/templateEstudiantesMaes.xlsx
+++ b/PosgrIQ/bin/Release/templates/templateEstudiantesMaes.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hdsp\Dropbox\Posgrados Ing Quimica\PosgrIQ\PosgrIQ\bin\Release\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PosgrIQ\PosgrIQ\bin\Release\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,17 +23,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>TABLA DE ESTUDIANTES DE MAESTRIA</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -48,12 +40,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Eras Bold ITC"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -89,21 +75,21 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -129,22 +115,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:colOff>3</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1701172</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>91442</xdr:rowOff>
+      <xdr:colOff>655812</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{413837E1-77DF-47CD-B7D7-40CD732D5FE0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -166,8 +152,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="180975" y="190500"/>
-          <a:ext cx="3215647" cy="853442"/>
+          <a:off x="180978" y="0"/>
+          <a:ext cx="2170284" cy="576000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -445,10 +431,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D23"/>
+  <dimension ref="A2:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B6" sqref="B1:B1048576"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,70 +454,152 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D2" s="3"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B8" s="6"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="6"/>
     </row>
     <row r="10" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7"/>
-      <c r="C10" s="5"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="7"/>
-      <c r="C13" s="6"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="7"/>
-      <c r="C15" s="6"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="7"/>
-      <c r="C16" s="6"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" s="7"/>
-      <c r="C17" s="6"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="7"/>
-      <c r="C18" s="6"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="7"/>
-      <c r="C19" s="6"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B20" s="7"/>
-      <c r="C20" s="6"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="7"/>
-      <c r="C21" s="6"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="7"/>
-      <c r="C22" s="6"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="7"/>
-      <c r="C23" s="6"/>
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="6"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="6"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="6"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="6"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="6"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="6"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="6"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="6"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="6"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="6"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="6"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="6"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="6"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="6"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="6"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="6"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="6"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.23622047244094491" right="5.7480314960629926" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>